<commit_message>
Updated imagestorage file to insert datas into database
</commit_message>
<xml_diff>
--- a/021/021/Product Data.xlsx
+++ b/021/021/Product Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Product"/>
@@ -549,7 +549,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -567,12 +567,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -604,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="18">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -651,23 +645,11 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -973,16 +955,16 @@
   </sheetPr>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="18" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="19" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="20" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="20" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="20" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="21" width="30.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="16" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="17" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="18.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="26.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="30.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
@@ -1205,7 +1187,7 @@
         <v>249</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1225,7 +1207,7 @@
         <v>299</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="33.75" customFormat="1" s="1">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1245,7 +1227,7 @@
         <v>269</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="47.25" customFormat="1" s="1">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1265,7 +1247,7 @@
         <v>209</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="47.25" customFormat="1" s="1">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -1285,7 +1267,7 @@
         <v>199</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="47.25" customFormat="1" s="1">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1305,7 +1287,7 @@
         <v>229</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="47.25" customFormat="1" s="1">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1325,7 +1307,7 @@
         <v>279</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="47.25" customFormat="1" s="1">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -1345,7 +1327,7 @@
         <v>189</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="47.25" customFormat="1" s="1">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -1365,7 +1347,7 @@
         <v>159</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -1385,7 +1367,7 @@
         <v>109</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -1405,7 +1387,7 @@
         <v>109</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="47.25" customFormat="1" s="1">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -1425,7 +1407,7 @@
         <v>199</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="33.75" customFormat="1" s="1">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -1445,12 +1427,12 @@
         <v>259</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="4">
         <v>23</v>
       </c>
       <c r="B24" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>122</v>
@@ -1465,12 +1447,12 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="4">
         <v>24</v>
       </c>
       <c r="B25" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>122</v>
@@ -1485,12 +1467,12 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="4">
         <v>25</v>
       </c>
       <c r="B26" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>122</v>
@@ -1505,12 +1487,12 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="4">
         <v>26</v>
       </c>
       <c r="B27" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>122</v>
@@ -1525,12 +1507,12 @@
         <v>48</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="4">
         <v>27</v>
       </c>
       <c r="B28" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>122</v>
@@ -1545,12 +1527,12 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="4">
         <v>28</v>
       </c>
       <c r="B29" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>122</v>
@@ -1565,12 +1547,12 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="4">
         <v>29</v>
       </c>
       <c r="B30" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>130</v>
@@ -1585,12 +1567,12 @@
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="4">
         <v>30</v>
       </c>
       <c r="B31" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>130</v>
@@ -1605,12 +1587,12 @@
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="4">
         <v>31</v>
       </c>
       <c r="B32" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>130</v>
@@ -1625,12 +1607,12 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="4">
         <v>32</v>
       </c>
       <c r="B33" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>130</v>
@@ -1645,12 +1627,12 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="4">
         <v>33</v>
       </c>
       <c r="B34" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>130</v>
@@ -1665,29 +1647,29 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A35" s="14"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="16"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="B35" s="4"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A36" s="14"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="16"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="B36" s="4"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A37" s="14"/>
-      <c r="B37" s="16"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="16"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4047,7 +4029,7 @@
   </sheetPr>
   <dimension ref="A1:D617"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
fixed the route of the BannerwithCarousel
</commit_message>
<xml_diff>
--- a/021/021/Product Data.xlsx
+++ b/021/021/Product Data.xlsx
@@ -967,7 +967,7 @@
     <col min="6" max="6" style="8" width="30.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -987,7 +987,7 @@
         <v>121</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>269</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>249</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>150</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>249</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>359</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>269</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>259</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>249</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>219</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>299</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="33.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>269</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="47.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>209</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="47.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>199</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="47.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>229</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="47.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>279</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="47.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>189</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="47.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A19" s="4">
         <v>18</v>
       </c>

</xml_diff>